<commit_message>
Split exported xlsx into sheets by year
</commit_message>
<xml_diff>
--- a/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
+++ b/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="4" r:id="rId1"/>
+    <sheet name="template" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
@@ -411,7 +411,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" sqref="A1:A2"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fill months in xlsx with empty savings
</commit_message>
<xml_diff>
--- a/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
+++ b/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
@@ -50,27 +50,37 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF385623"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF385623"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -99,7 +109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -148,11 +158,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color theme="3" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -177,6 +202,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -187,7 +230,12 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -195,6 +243,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -411,24 +464,28 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.19921875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="12.59765625" style="2"/>
+    <col min="3" max="3" width="14.8984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.59765625" style="2"/>
+    <col min="5" max="5" width="14.8984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="12.59765625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -460,11 +517,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>44562</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <f>SUM(B5:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <f>SUM(D5:D5)</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <f>(C5-E5) + IF(F4 ="", F3, F4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
@@ -1185,6 +1261,11 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <conditionalFormatting sqref="F4">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Refactor xlsx parsing, services and entities
</commit_message>
<xml_diff>
--- a/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
+++ b/backend/backend-app/src/main/resources/xlsx/generation-template.xlsx
@@ -77,7 +77,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF385623"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -196,9 +196,6 @@
     <xf numFmtId="43" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -217,13 +214,16 @@
     <xf numFmtId="43" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,7 +464,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -479,17 +479,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1"/>
@@ -512,30 +512,30 @@
         <f>SUM(D4:D4)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="16">
         <f>(C4-E4) + IF(F3 ="", F2, F3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>44562</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f>SUM(B5:B5)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <f>SUM(D5:D5)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="17">
         <f>(C5-E5) + IF(F4 ="", F3, F4)</f>
         <v>0</v>
       </c>

</xml_diff>